<commit_message>
fixed major bugs in assembler, circuit and control signal mappings.
</commit_message>
<xml_diff>
--- a/CONTROL_MAPPINGS.xlsx
+++ b/CONTROL_MAPPINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722495F6-BC69-4418-9C8E-5305C8925D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD54A1F-DC67-44BF-AD7D-DE7BC0AF7786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="B2:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +695,7 @@
         <v>37</v>
       </c>
       <c r="G3" s="4">
-        <f>IF(AND(OR(F3="R", F3="I"),  NOT(E3="lw")), 1, 0)</f>
+        <f>IF(AND(OR(F3="R", E3="sw"), NOT(E3="sll"),  NOT(E3="srl")), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="H3" s="4">
@@ -707,39 +707,39 @@
         <v>0</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J3:J17" si="1">IF(OR(F5="I", F5="R", E5="lw"), 1, 0)</f>
+        <f>IF(AND(OR(F3="I", F3="R", E3="lw"), NOT(E3="sw"), NOT(E3="beq"), NOT(E3="bneq")), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K18" si="2">IF(E3="lw", 1, 0)</f>
+        <f t="shared" ref="K3:K18" si="1">IF(E3="lw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L18" si="3">IF(E3="sw", 1, 0)</f>
+        <f t="shared" ref="L3:L18" si="2">IF(E3="sw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" ref="M3:M18" si="4">IF(E3="beq", 1, 0)</f>
+        <f t="shared" ref="M3:M18" si="3">IF(E3="beq", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N18" si="5">IF(E3="bneq", 1, 0)</f>
+        <f t="shared" ref="N3:N18" si="4">IF(E3="bneq", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="O3" s="4">
-        <f t="shared" ref="O3:O18" si="6">IF(E3="j", 1, 0)</f>
+        <f t="shared" ref="O3:O18" si="5">IF(E3="j", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P3" s="5">
-        <f t="shared" ref="P3:P18" si="7">IF(OR(TRIM(E3)="nor", TRIM(E3)="sll", TRIM(E3)="srl", TRIM(E3)="sra"), 1, 0)</f>
+        <f t="shared" ref="P3:P18" si="6">IF(OR(TRIM(E3)="nor", TRIM(E3)="sll", TRIM(E3)="srl", TRIM(E3)="sra"), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q18" si="8">IF(OR(TRIM(E3)="or", TRIM(E3)="and", TRIM(E3)="srl", TRIM(E3)="sra", TRIM(E3)="ori", TRIM(E3)="andi"), 1, 0)</f>
+        <f t="shared" ref="Q3:Q18" si="7">IF(OR(TRIM(E3)="or", TRIM(E3)="and", TRIM(E3)="srl", TRIM(E3)="sra", TRIM(E3)="ori", TRIM(E3)="andi"), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R3" s="5">
-        <f t="shared" ref="R3:R18" si="9">IF(OR(TRIM(E3)="sub", TRIM(E3)="subi", TRIM(E3)="and", TRIM(E3)="andi", TRIM(E3)="sll", TRIM(E3)="sra"), 1, 0)</f>
+        <f>IF(OR(TRIM(E3)="sub", TRIM(E3)="subi", TRIM(E3)="and", TRIM(E3)="andi", TRIM(E3)="sll", TRIM(E3)="sra", TRIM(E3)="bneq", TRIM(E3)="beq"), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S3" s="3" t="str">
@@ -772,11 +772,11 @@
         <v>37</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G18" si="10">IF(AND(OR(F4="R", F4="I"),  NOT(E4="lw")), 1, 0)</f>
-        <v>1</v>
+        <f t="shared" ref="G4:G18" si="8">IF(AND(OR(F4="R", E4="sw"), NOT(E4="sll"),  NOT(E4="srl")), 1, 0)</f>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H18" si="11">IF(OR(E4="lw", E4="sw", E4="andi", E4="ori", E4="addi", E4="subi", E4="sll", E4="srl"), 1, 0)</f>
+        <f t="shared" ref="H4:H18" si="9">IF(OR(E4="lw", E4="sw", E4="andi", E4="ori", E4="addi", E4="subi", E4="sll", E4="srl"), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I4" s="4">
@@ -784,52 +784,52 @@
         <v>0</v>
       </c>
       <c r="J4" s="4">
+        <f t="shared" ref="J4:J18" si="10">IF(AND(OR(F4="I", F4="R", E4="lw"), NOT(E4="sw"), NOT(E4="beq"), NOT(E4="bneq")), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
       <c r="R4" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="R4:R18" si="11">IF(OR(TRIM(E4)="sub", TRIM(E4)="subi", TRIM(E4)="and", TRIM(E4)="andi", TRIM(E4)="sll", TRIM(E4)="sra", TRIM(E4)="bneq", TRIM(E4)="beq"), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S4" s="3" t="str">
         <f t="shared" ref="S4:S18" si="12">_xlfn.TEXTJOIN("", TRUE, G4:R4)</f>
-        <v>110100000110</v>
+        <v>010100000110</v>
       </c>
       <c r="T4">
         <f t="shared" ref="T4:T18" ca="1" si="13">SUMPRODUCT(MID(S4,LEN(S4)-ROW(INDIRECT("1:"&amp;LEN(S4)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(S4)))-1))</f>
-        <v>3334</v>
+        <v>1286</v>
       </c>
       <c r="U4" s="2" t="str">
         <f t="shared" ref="U4:U18" ca="1" si="14">DEC2HEX(T4)</f>
-        <v>D06</v>
+        <v>506</v>
       </c>
       <c r="W4" s="13" t="s">
         <v>47</v>
@@ -857,11 +857,11 @@
         <v>38</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I5" s="4">
@@ -869,52 +869,52 @@
         <v>0</v>
       </c>
       <c r="J5" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="S5" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>110100000011</v>
+        <v>010100000011</v>
       </c>
       <c r="T5">
         <f t="shared" ca="1" si="13"/>
-        <v>3331</v>
+        <v>1283</v>
       </c>
       <c r="U5" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>D03</v>
+        <v>503</v>
       </c>
       <c r="W5" t="s">
         <v>54</v>
@@ -946,11 +946,11 @@
         <v>38</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I6" s="4">
@@ -958,55 +958,55 @@
         <v>0</v>
       </c>
       <c r="J6" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S6" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>110100000010</v>
+        <v>010100000010</v>
       </c>
       <c r="T6">
         <f t="shared" ca="1" si="13"/>
-        <v>3330</v>
+        <v>1282</v>
       </c>
       <c r="U6" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>D02</v>
+        <v>502</v>
       </c>
       <c r="W6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="X6" s="11">
         <v>1</v>
@@ -1035,11 +1035,11 @@
         <v>37</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I7" s="4">
@@ -1047,39 +1047,39 @@
         <v>0</v>
       </c>
       <c r="J7" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S7" s="3" t="str">
@@ -1095,7 +1095,7 @@
         <v>904</v>
       </c>
       <c r="W7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X7" s="11">
         <v>10</v>
@@ -1124,11 +1124,11 @@
         <v>38</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I8" s="4">
@@ -1136,55 +1136,55 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P8" s="5">
+      <c r="Q8" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R8" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="S8" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>100100010000</v>
+        <v>000000010001</v>
       </c>
       <c r="T8">
         <f t="shared" ca="1" si="13"/>
-        <v>2320</v>
+        <v>17</v>
       </c>
       <c r="U8" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>910</v>
+        <v>11</v>
       </c>
       <c r="W8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X8" s="11">
         <v>11</v>
@@ -1213,11 +1213,11 @@
         <v>37</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I9" s="4">
@@ -1225,39 +1225,39 @@
         <v>0</v>
       </c>
       <c r="J9" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="S9" s="3" t="str">
@@ -1273,7 +1273,7 @@
         <v>903</v>
       </c>
       <c r="W9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="X9" s="11">
         <v>100</v>
@@ -1302,11 +1302,11 @@
         <v>38</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I10" s="4">
@@ -1314,52 +1314,52 @@
         <v>0</v>
       </c>
       <c r="J10" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P10" s="5">
+      <c r="Q10" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R10" s="5">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="S10" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>100100100000</v>
+        <v>000000100001</v>
       </c>
       <c r="T10">
         <f t="shared" ca="1" si="13"/>
-        <v>2336</v>
+        <v>33</v>
       </c>
       <c r="U10" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>920</v>
+        <v>21</v>
       </c>
       <c r="W10" t="s">
         <v>48</v>
@@ -1391,11 +1391,11 @@
         <v>38</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I11" s="4">
@@ -1403,52 +1403,52 @@
         <v>1</v>
       </c>
       <c r="J11" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O11" s="4">
+      <c r="P11" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P11" s="5">
+      <c r="Q11" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S11" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>111101000000</v>
+        <v>111001000000</v>
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="13"/>
-        <v>3904</v>
+        <v>3648</v>
       </c>
       <c r="U11" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>F40</v>
+        <v>E40</v>
       </c>
       <c r="W11" t="s">
         <v>53</v>
@@ -1480,11 +1480,11 @@
         <v>38</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I12" s="4">
@@ -1492,52 +1492,52 @@
         <v>0</v>
       </c>
       <c r="J12" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R12" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="S12" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>110100000001</v>
+        <v>010100000001</v>
       </c>
       <c r="T12">
         <f t="shared" ca="1" si="13"/>
-        <v>3329</v>
+        <v>1281</v>
       </c>
       <c r="U12" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>D01</v>
+        <v>501</v>
       </c>
       <c r="Y12" s="10">
         <v>111</v>
@@ -1563,11 +1563,11 @@
         <v>38</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I13" s="4">
@@ -1575,52 +1575,52 @@
         <v>0</v>
       </c>
       <c r="J13" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P13" s="5">
+      <c r="Q13" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R13" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S13" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>110100000000</v>
+        <v>010100000000</v>
       </c>
       <c r="T13">
         <f t="shared" ca="1" si="13"/>
-        <v>3328</v>
+        <v>1280</v>
       </c>
       <c r="U13" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>D00</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.3">
@@ -1640,11 +1640,11 @@
         <v>37</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I14" s="4">
@@ -1652,52 +1652,52 @@
         <v>0</v>
       </c>
       <c r="J14" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="5">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R14" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="S14" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>110100000101</v>
+        <v>010100000101</v>
       </c>
       <c r="T14">
         <f t="shared" ca="1" si="13"/>
-        <v>3333</v>
+        <v>1285</v>
       </c>
       <c r="U14" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>D05</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.3">
@@ -1717,11 +1717,11 @@
         <v>37</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I15" s="4">
@@ -1729,39 +1729,39 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="M15" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O15" s="4">
+      <c r="P15" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R15" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S15" s="3" t="str">
@@ -1794,11 +1794,11 @@
         <v>38</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I16" s="4">
@@ -1806,52 +1806,52 @@
         <v>0</v>
       </c>
       <c r="J16" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P16" s="5">
+      <c r="Q16" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R16" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S16" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>010010000000</v>
+        <v>010110000000</v>
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="13"/>
-        <v>1152</v>
+        <v>1408</v>
       </c>
       <c r="U16" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>480</v>
+        <v>580</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
@@ -1871,11 +1871,11 @@
         <v>37</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I17" s="4">
@@ -1883,52 +1883,52 @@
         <v>0</v>
       </c>
       <c r="J17" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="M17" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N17" s="4">
+      <c r="O17" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P17" s="5">
+      <c r="Q17" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R17" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S17" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>100000000010</v>
+        <v>100100000010</v>
       </c>
       <c r="T17">
         <f t="shared" ca="1" si="13"/>
-        <v>2050</v>
+        <v>2306</v>
       </c>
       <c r="U17" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>802</v>
+        <v>902</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>39</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I18" s="4">
@@ -1960,39 +1960,39 @@
         <v>0</v>
       </c>
       <c r="J18" s="4">
-        <f>IF(OR(F21="I", F21="R", E21="lw"), 1, 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K18" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L18" s="4">
+      <c r="M18" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N18" s="4">
+      <c r="O18" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="5">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="R18" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S18" s="3" t="str">
@@ -2015,7 +2015,7 @@
       <c r="U20" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("v2.0 raw", CHAR(10), _xlfn.TEXTJOIN(" ", TRUE, U3:U18))</f>
         <v>v2.0 raw
-901 D06 D03 D02 904 910 903 920 F40 D01 D00 D05 900 480 802 8</v>
+901 506 503 502 904 11 903 21 E40 501 500 505 900 580 902 8</v>
       </c>
     </row>
     <row r="21" spans="2:21" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed whole MIPS. completed full set opcode test of mips.
</commit_message>
<xml_diff>
--- a/CONTROL_MAPPINGS.xlsx
+++ b/CONTROL_MAPPINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD54A1F-DC67-44BF-AD7D-DE7BC0AF7786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F718F6-5A50-457A-8E21-FE7C083417B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,7 +192,7 @@
     <t>$zero</t>
   </si>
   <si>
-    <t xml:space="preserve">update this column according to your group </t>
+    <t>update this column if series changes</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="B2:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I18" si="0">IF(E3="sw", 1, 0)</f>
+        <f>IF(E3="lw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J3" s="4">
@@ -711,31 +711,31 @@
         <v>1</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K18" si="1">IF(E3="lw", 1, 0)</f>
+        <f t="shared" ref="K3:K18" si="0">IF(E3="lw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L18" si="2">IF(E3="sw", 1, 0)</f>
+        <f t="shared" ref="L3:L18" si="1">IF(E3="sw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" ref="M3:M18" si="3">IF(E3="beq", 1, 0)</f>
+        <f t="shared" ref="M3:M18" si="2">IF(E3="beq", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N18" si="4">IF(E3="bneq", 1, 0)</f>
+        <f t="shared" ref="N3:N18" si="3">IF(E3="bneq", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="O3" s="4">
-        <f t="shared" ref="O3:O18" si="5">IF(E3="j", 1, 0)</f>
+        <f t="shared" ref="O3:O18" si="4">IF(E3="j", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P3" s="5">
-        <f t="shared" ref="P3:P18" si="6">IF(OR(TRIM(E3)="nor", TRIM(E3)="sll", TRIM(E3)="srl", TRIM(E3)="sra"), 1, 0)</f>
+        <f t="shared" ref="P3:P18" si="5">IF(OR(TRIM(E3)="nor", TRIM(E3)="sll", TRIM(E3)="srl", TRIM(E3)="sra"), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q18" si="7">IF(OR(TRIM(E3)="or", TRIM(E3)="and", TRIM(E3)="srl", TRIM(E3)="sra", TRIM(E3)="ori", TRIM(E3)="andi"), 1, 0)</f>
+        <f t="shared" ref="Q3:Q18" si="6">IF(OR(TRIM(E3)="or", TRIM(E3)="and", TRIM(E3)="srl", TRIM(E3)="sra", TRIM(E3)="ori", TRIM(E3)="andi"), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R3" s="5">
@@ -772,15 +772,15 @@
         <v>37</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G18" si="8">IF(AND(OR(F4="R", E4="sw"), NOT(E4="sll"),  NOT(E4="srl")), 1, 0)</f>
+        <f t="shared" ref="G4:G18" si="7">IF(AND(OR(F4="R", E4="sw"), NOT(E4="sll"),  NOT(E4="srl")), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H18" si="9">IF(OR(E4="lw", E4="sw", E4="andi", E4="ori", E4="addi", E4="subi", E4="sll", E4="srl"), 1, 0)</f>
+        <f t="shared" ref="H4:H18" si="8">IF(OR(E4="lw", E4="sw", E4="andi", E4="ori", E4="addi", E4="subi", E4="sll", E4="srl"), 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I4:I18" si="9">IF(E4="lw", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J4" s="4">
@@ -788,31 +788,31 @@
         <v>1</v>
       </c>
       <c r="K4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R4" s="5">
@@ -857,15 +857,15 @@
         <v>38</v>
       </c>
       <c r="G5" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="4">
@@ -873,31 +873,31 @@
         <v>1</v>
       </c>
       <c r="K5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R5" s="5">
@@ -946,15 +946,15 @@
         <v>38</v>
       </c>
       <c r="G6" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6" s="4">
@@ -962,31 +962,31 @@
         <v>1</v>
       </c>
       <c r="K6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R6" s="5">
@@ -1035,15 +1035,15 @@
         <v>37</v>
       </c>
       <c r="G7" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7" s="4">
@@ -1051,31 +1051,31 @@
         <v>1</v>
       </c>
       <c r="K7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R7" s="5">
@@ -1124,15 +1124,15 @@
         <v>38</v>
       </c>
       <c r="G8" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="4">
@@ -1140,31 +1140,31 @@
         <v>0</v>
       </c>
       <c r="K8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P8" s="5">
+      <c r="Q8" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R8" s="5">
@@ -1213,15 +1213,15 @@
         <v>37</v>
       </c>
       <c r="G9" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="4">
@@ -1229,31 +1229,31 @@
         <v>1</v>
       </c>
       <c r="K9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R9" s="5">
@@ -1302,15 +1302,15 @@
         <v>38</v>
       </c>
       <c r="G10" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10" s="4">
@@ -1318,31 +1318,31 @@
         <v>0</v>
       </c>
       <c r="K10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P10" s="5">
+      <c r="Q10" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R10" s="5">
@@ -1391,47 +1391,47 @@
         <v>38</v>
       </c>
       <c r="G11" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O11" s="4">
+      <c r="P11" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P11" s="5">
+      <c r="Q11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R11" s="5">
@@ -1440,15 +1440,15 @@
       </c>
       <c r="S11" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>111001000000</v>
+        <v>110001000000</v>
       </c>
       <c r="T11">
         <f t="shared" ca="1" si="13"/>
-        <v>3648</v>
+        <v>3136</v>
       </c>
       <c r="U11" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>E40</v>
+        <v>C40</v>
       </c>
       <c r="W11" t="s">
         <v>53</v>
@@ -1480,15 +1480,15 @@
         <v>38</v>
       </c>
       <c r="G12" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="4">
@@ -1496,31 +1496,31 @@
         <v>1</v>
       </c>
       <c r="K12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R12" s="5">
@@ -1563,15 +1563,15 @@
         <v>38</v>
       </c>
       <c r="G13" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="4">
@@ -1579,31 +1579,31 @@
         <v>1</v>
       </c>
       <c r="K13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P13" s="5">
+      <c r="Q13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R13" s="5">
@@ -1640,15 +1640,15 @@
         <v>37</v>
       </c>
       <c r="G14" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="4">
@@ -1656,31 +1656,31 @@
         <v>1</v>
       </c>
       <c r="K14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="5">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R14" s="5">
@@ -1717,15 +1717,15 @@
         <v>37</v>
       </c>
       <c r="G15" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="4">
@@ -1733,31 +1733,31 @@
         <v>1</v>
       </c>
       <c r="K15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="M15" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O15" s="4">
+      <c r="P15" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R15" s="5">
@@ -1794,47 +1794,47 @@
         <v>38</v>
       </c>
       <c r="G16" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
         <f t="shared" si="9"/>
         <v>1</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="K16" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P16" s="5">
+      <c r="Q16" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R16" s="5">
@@ -1843,15 +1843,15 @@
       </c>
       <c r="S16" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>010110000000</v>
+        <v>011110000000</v>
       </c>
       <c r="T16">
         <f t="shared" ca="1" si="13"/>
-        <v>1408</v>
+        <v>1920</v>
       </c>
       <c r="U16" s="2" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>580</v>
+        <v>780</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
@@ -1871,15 +1871,15 @@
         <v>37</v>
       </c>
       <c r="G17" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="4">
@@ -1887,31 +1887,31 @@
         <v>1</v>
       </c>
       <c r="K17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="M17" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17" s="4">
+      <c r="O17" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P17" s="5">
+      <c r="Q17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R17" s="5">
@@ -1948,15 +1948,15 @@
         <v>39</v>
       </c>
       <c r="G18" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H18" s="4">
+      <c r="I18" s="4">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18" s="4">
@@ -1964,31 +1964,31 @@
         <v>0</v>
       </c>
       <c r="K18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L18" s="4">
+      <c r="M18" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N18" s="4">
+      <c r="O18" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="5">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R18" s="5">
@@ -2015,7 +2015,7 @@
       <c r="U20" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("v2.0 raw", CHAR(10), _xlfn.TEXTJOIN(" ", TRUE, U3:U18))</f>
         <v>v2.0 raw
-901 506 503 502 904 11 903 21 E40 501 500 505 900 580 902 8</v>
+901 506 503 502 904 11 903 21 C40 501 500 505 900 780 902 8</v>
       </c>
     </row>
     <row r="21" spans="2:21" ht="57.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed updated alu .jar bug.
</commit_message>
<xml_diff>
--- a/CONTROL_MAPPINGS.xlsx
+++ b/CONTROL_MAPPINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F718F6-5A50-457A-8E21-FE7C083417B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C9849D-DB4E-44B9-AD36-F258416966F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="B2:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
TESTED BASIC PIPELINE [PASSED]
</commit_message>
<xml_diff>
--- a/CONTROL_MAPPINGS.xlsx
+++ b/CONTROL_MAPPINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C9849D-DB4E-44B9-AD36-F258416966F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B60EB5D-C64C-4DE4-8D38-E76BD28B3901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>REG-DEST | ALU-SRC | MEM-TO-REG | REG-WRITE | MEM-READ | MEM-WRITE | BEQ | BNEQ | JUMP | ALUOP</t>
   </si>
   <si>
-    <t>register mapping</t>
-  </si>
-  <si>
     <t>$t0</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>update this column if series changes</t>
+  </si>
+  <si>
+    <t>Register mapping</t>
   </si>
 </sst>
 </file>
@@ -313,14 +313,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,7 +605,7 @@
   <dimension ref="B2:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="W4" sqref="W4:X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,11 +663,11 @@
       <c r="O2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
       <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
@@ -831,14 +831,14 @@
         <f t="shared" ref="U4:U18" ca="1" si="14">DEC2HEX(T4)</f>
         <v>506</v>
       </c>
-      <c r="W4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13" t="s">
+      <c r="W4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Z4" s="13"/>
+      <c r="Z4" s="12"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B5">
@@ -917,7 +917,7 @@
         <v>503</v>
       </c>
       <c r="W5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X5" s="11">
         <v>0</v>
@@ -1006,7 +1006,7 @@
         <v>502</v>
       </c>
       <c r="W6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X6" s="11">
         <v>1</v>
@@ -1095,7 +1095,7 @@
         <v>904</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X7" s="11">
         <v>10</v>
@@ -1184,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="W8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X8" s="11">
         <v>11</v>
@@ -1273,7 +1273,7 @@
         <v>903</v>
       </c>
       <c r="W9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X9" s="11">
         <v>100</v>
@@ -1362,7 +1362,7 @@
         <v>21</v>
       </c>
       <c r="W10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="X10" s="11">
         <v>101</v>
@@ -1451,7 +1451,7 @@
         <v>C40</v>
       </c>
       <c r="W11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X11" s="11">
         <v>110</v>
@@ -2009,9 +2009,10 @@
       </c>
     </row>
     <row r="20" spans="2:21" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="E20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="14"/>
       <c r="U20" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("v2.0 raw", CHAR(10), _xlfn.TEXTJOIN(" ", TRUE, U3:U18))</f>
         <v>v2.0 raw
@@ -2024,74 +2025,74 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
       <c r="U23" s="6"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="B26:S26"/>
@@ -2099,6 +2100,7 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:S25"/>
     <mergeCell ref="W4:X4"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IO peripheral done. Working display adapter and display unit. Made and tested a random unit. Wrote random matrix code.
</commit_message>
<xml_diff>
--- a/CONTROL_MAPPINGS.xlsx
+++ b/CONTROL_MAPPINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B60EB5D-C64C-4DE4-8D38-E76BD28B3901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBEBEB4-1137-4936-ACA4-A66D8F4E35B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Z26"/>
+  <dimension ref="B2:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:X4"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,9 +618,10 @@
     <col min="19" max="19" width="19.88671875" customWidth="1"/>
     <col min="20" max="20" width="11.109375" customWidth="1"/>
     <col min="21" max="21" width="19.109375" customWidth="1"/>
+    <col min="28" max="29" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -678,7 +679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -755,7 +756,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -839,8 +840,10 @@
         <v>45</v>
       </c>
       <c r="Z4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -929,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>13</v>
       </c>
@@ -2092,7 +2095,8 @@
       <c r="S26" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="B26:S26"/>

</xml_diff>